<commit_message>
partly implemented a sweep algorithm
</commit_message>
<xml_diff>
--- a/WGUPS Package File.xlsx
+++ b/WGUPS Package File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Dropbox\WGU\Courses\C950\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8D63FB2-6AE6-4811-906E-876A28FCBF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E788974-13D2-4ABA-8A25-8B1E587FA0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57630" yWindow="30" windowWidth="21600" windowHeight="29565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$8:$H$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -309,18 +308,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -336,6 +323,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,12 +673,12 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="20"/>
+    <col min="1" max="1" width="8.85546875" style="16"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
@@ -689,82 +688,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="13"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="A2" s="13"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -790,158 +789,156 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="15">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G9" s="10">
+        <v>21</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10">
+        <v>84106</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="10">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+    </row>
+    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="10">
+        <v>84111</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="10">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" s="21" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>6</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="G9" s="10">
-        <v>4</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="C14" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12">
+        <v>84119</v>
+      </c>
+      <c r="F14" s="19">
         <v>0.4375</v>
       </c>
-      <c r="G10" s="10">
-        <v>21</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>6</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12">
-        <v>84119</v>
-      </c>
-      <c r="F11" s="23">
-        <v>0.4375</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="G14" s="12">
         <v>88</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H14" s="20" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>13</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10">
-        <v>84104</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>14</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="G13" s="10">
-        <v>88</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="25" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>16</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="G14" s="10">
-        <v>88</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -950,11 +947,11 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>20</v>
+      <c r="A15" s="15">
+        <v>7</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>7</v>
@@ -963,50 +960,46 @@
         <v>8</v>
       </c>
       <c r="E15" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F15" s="11">
-        <v>0.4375</v>
+        <v>84106</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G15" s="10">
-        <v>37</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="25" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>25</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="12">
-        <v>84117</v>
-      </c>
-      <c r="F16" s="23">
-        <v>0.4375</v>
-      </c>
-      <c r="G16" s="12">
-        <v>7</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>17</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" s="21" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="10">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>29</v>
+      <c r="A17" s="15">
+        <v>9</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>7</v>
@@ -1015,22 +1008,24 @@
         <v>8</v>
       </c>
       <c r="E17" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0.4375</v>
+        <v>84103</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G17" s="10">
         <v>2</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>30</v>
+      <c r="A18" s="15">
+        <v>10</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -1039,10 +1034,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0.4375</v>
+        <v>84105</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -1050,11 +1045,11 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>31</v>
+      <c r="A19" s="15">
+        <v>11</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>7</v>
@@ -1063,10 +1058,10 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0.4375</v>
+        <v>84118</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -1074,35 +1069,35 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>34</v>
+      <c r="A20" s="15">
+        <v>12</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.4375</v>
+        <v>84119</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G20" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <v>37</v>
+      <c r="A21" s="15">
+        <v>13</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
@@ -1111,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="10">
-        <v>84111</v>
+        <v>84104</v>
       </c>
       <c r="F21" s="11">
         <v>0.4375</v>
@@ -1122,231 +1117,235 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
-        <v>40</v>
+      <c r="A22" s="15">
+        <v>14</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="10">
-        <v>84115</v>
+        <v>84117</v>
       </c>
       <c r="F22" s="11">
         <v>0.4375</v>
       </c>
       <c r="G22" s="10">
-        <v>45</v>
-      </c>
-      <c r="H22" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="15">
+        <v>15</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="10">
+        <v>84117</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="G23" s="10">
+        <v>4</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>16</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="10">
+        <v>84117</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G24" s="10">
+        <v>88</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>17</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="10">
+        <v>84119</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="10">
         <v>2</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="10">
-        <v>44</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>18</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="10">
+        <v>84123</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="10">
+        <v>6</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>19</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="10">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>20</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G28" s="10">
+        <v>37</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>21</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="10">
         <v>3</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="10">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>22</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10">
+        <v>84121</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="10">
         <v>2</v>
       </c>
-      <c r="H24" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
-        <v>4</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="10">
-        <v>4</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
-        <v>5</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="10">
-        <v>84111</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="10">
-        <v>5</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
-        <v>7</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="10">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
-        <v>8</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="10">
-        <v>9</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
-        <v>9</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="10">
-        <v>2</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
-        <v>10</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="10">
-        <v>84105</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1</v>
-      </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
-        <v>11</v>
+      <c r="A31" s="15">
+        <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -1361,64 +1360,66 @@
         <v>10</v>
       </c>
       <c r="G31" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
-        <v>12</v>
+      <c r="A32" s="15">
+        <v>24</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="10">
-        <v>84119</v>
+        <v>84107</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
+      <c r="A33" s="12">
+        <v>25</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="12">
+        <v>84117</v>
+      </c>
+      <c r="F33" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="G33" s="12">
+        <v>7</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="10">
-        <v>2</v>
-      </c>
-      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
-        <v>18</v>
+      <c r="A34" s="15">
+        <v>26</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -1427,24 +1428,22 @@
         <v>8</v>
       </c>
       <c r="E34" s="10">
-        <v>84123</v>
+        <v>84117</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="10">
-        <v>6</v>
-      </c>
-      <c r="H34" s="21" t="s">
-        <v>12</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
-        <v>19</v>
+      <c r="A35" s="15">
+        <v>27</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -1453,22 +1452,22 @@
         <v>8</v>
       </c>
       <c r="E35" s="10">
-        <v>84115</v>
+        <v>84104</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="10">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
-        <v>21</v>
+      <c r="A36" s="15">
+        <v>28</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -1483,28 +1482,30 @@
         <v>10</v>
       </c>
       <c r="G36" s="10">
-        <v>3</v>
-      </c>
-      <c r="H36" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
-        <v>22</v>
+      <c r="A37" s="15">
+        <v>29</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="10">
-        <v>84121</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>10</v>
+        <v>84106</v>
+      </c>
+      <c r="F37" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G37" s="10">
         <v>2</v>
@@ -1512,242 +1513,242 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="A38" s="15">
+        <v>30</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F38" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>31</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="10">
+        <v>84119</v>
+      </c>
+      <c r="F39" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G39" s="10">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>32</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="10">
+        <v>84119</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="10">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>33</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="10">
+        <v>84106</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="10">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>34</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="10">
+        <v>84117</v>
+      </c>
+      <c r="F42" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G42" s="10">
+        <v>2</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>35</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="10">
+        <v>84104</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="10">
+        <v>88</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>36</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="10">
+        <v>84119</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="10">
+        <v>88</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>37</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="10">
+        <v>84111</v>
+      </c>
+      <c r="F45" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G45" s="10">
+        <v>2</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>38</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="10">
+        <v>84111</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="10">
+        <v>9</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>39</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="10">
-        <v>84118</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="10">
-        <v>5</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
-        <v>24</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="10">
-        <v>84107</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="10">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
-        <v>26</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="10">
-        <v>25</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19">
-        <v>27</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="10">
+      <c r="C47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="10">
         <v>84104</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="10">
-        <v>5</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
-        <v>28</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="10">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
-        <v>32</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="10">
-        <v>1</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
-        <v>33</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="10">
-        <v>1</v>
-      </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
-        <v>35</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="10">
-        <v>84104</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="10">
-        <v>88</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
-        <v>36</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="10">
-        <v>88</v>
-      </c>
-      <c r="H46" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19">
-        <v>38</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="10">
-        <v>84111</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>10</v>
@@ -1755,16 +1756,14 @@
       <c r="G47" s="10">
         <v>9</v>
       </c>
-      <c r="H47" s="21" t="s">
-        <v>12</v>
-      </c>
+      <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
-        <v>39</v>
+      <c r="A48" s="15">
+        <v>40</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>7</v>
@@ -1773,20 +1772,20 @@
         <v>8</v>
       </c>
       <c r="E48" s="10">
-        <v>84104</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>10</v>
+        <v>84115</v>
+      </c>
+      <c r="F48" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G48" s="10">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="H48" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:H48" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H48">
-      <sortCondition ref="F8:F48"/>
+      <sortCondition ref="A8:A48"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:M22">
@@ -2242,15 +2241,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
@@ -2287,6 +2277,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A0206-F67A-481E-AE05-AF5EAD7E6628}">
   <ds:schemaRefs>
@@ -2308,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2331,4 +2322,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
need to add package affinity handler
</commit_message>
<xml_diff>
--- a/WGUPS Package File.xlsx
+++ b/WGUPS Package File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Dropbox\WGU\Courses\C950\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E788974-13D2-4ABA-8A25-8B1E587FA0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F4B58D-8E13-47B0-842F-7C23F535555D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1155" windowWidth="21600" windowHeight="29565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -326,15 +326,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,7 +674,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,40 +728,40 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
@@ -790,34 +791,34 @@
     </row>
     <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="10">
-        <v>84115</v>
+        <v>84117</v>
       </c>
       <c r="F9" s="11">
-        <v>0.4375</v>
+        <v>0.375</v>
       </c>
       <c r="G9" s="10">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>7</v>
@@ -826,53 +827,48 @@
         <v>8</v>
       </c>
       <c r="E10" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>10</v>
+        <v>84115</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G10" s="10">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
     </row>
     <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>3</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>12</v>
+      <c r="A11" s="12">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12">
+        <v>84119</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="G11" s="12">
+        <v>88</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>7</v>
@@ -881,64 +877,66 @@
         <v>8</v>
       </c>
       <c r="E12" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>10</v>
+        <v>84104</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G12" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="10">
-        <v>84111</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>10</v>
+        <v>84117</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G13" s="10">
-        <v>5</v>
-      </c>
-      <c r="H13" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:13" s="21" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>6</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="A14" s="15">
         <v>16</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="12">
-        <v>84119</v>
-      </c>
-      <c r="F14" s="19">
+      <c r="B14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="10">
+        <v>84117</v>
+      </c>
+      <c r="F14" s="11">
         <v>0.4375</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="10">
         <v>88</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>17</v>
+      <c r="H14" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -948,84 +946,101 @@
     </row>
     <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="10">
+        <v>84115</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="G15" s="10">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+    </row>
+    <row r="16" spans="1:13" s="21" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>25</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="12">
+        <v>84117</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="G16" s="12">
+        <v>7</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="C17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10">
         <v>84106</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="10">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" s="21" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
-        <v>8</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="10">
-        <v>9</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>9</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>10</v>
+      <c r="F17" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G17" s="10">
         <v>2</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="4"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -1034,22 +1049,22 @@
         <v>8</v>
       </c>
       <c r="E18" s="10">
-        <v>84105</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>10</v>
+        <v>84103</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>7</v>
@@ -1058,46 +1073,46 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>84118</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>10</v>
+        <v>84119</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>10</v>
+        <v>84117</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.4375</v>
       </c>
       <c r="G20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
@@ -1106,7 +1121,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="10">
-        <v>84104</v>
+        <v>84111</v>
       </c>
       <c r="F21" s="11">
         <v>0.4375</v>
@@ -1116,88 +1131,86 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="10">
-        <v>84117</v>
+        <v>84115</v>
       </c>
       <c r="F22" s="11">
         <v>0.4375</v>
       </c>
       <c r="G22" s="10">
-        <v>88</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0.375</v>
+        <v>84106</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G23" s="10">
+        <v>44</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>3</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="10">
+        <v>2</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <v>4</v>
       </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
-        <v>16</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="G24" s="10">
-        <v>88</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
-        <v>17</v>
-      </c>
       <c r="B25" s="9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>7</v>
@@ -1206,146 +1219,144 @@
         <v>8</v>
       </c>
       <c r="E25" s="10">
-        <v>84119</v>
+        <v>84115</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="10">
+        <v>4</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>5</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="10">
+        <v>84111</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="10">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>7</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="10">
+        <v>84106</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="10">
+        <v>8</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>8</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="10">
+        <v>9</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>9</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="10">
+        <v>84103</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="10">
         <v>2</v>
       </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
-        <v>18</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="10">
-        <v>84123</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="10">
-        <v>6</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
-        <v>19</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="10">
-        <v>37</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="H29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>10</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F28" s="11">
-        <v>0.4375</v>
-      </c>
-      <c r="G28" s="10">
-        <v>37</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="C30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10">
+        <v>84105</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="10">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>11</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="10">
-        <v>3</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
-        <v>22</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="10">
-        <v>84121</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="10">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
-        <v>23</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>7</v>
@@ -1360,66 +1371,64 @@
         <v>10</v>
       </c>
       <c r="G31" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="10">
-        <v>84107</v>
+        <v>84119</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>25</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="12">
-        <v>84117</v>
-      </c>
-      <c r="F33" s="19">
-        <v>0.4375</v>
-      </c>
-      <c r="G33" s="12">
-        <v>7</v>
-      </c>
-      <c r="H33" s="20" t="s">
+      <c r="A33" s="15">
         <v>17</v>
       </c>
+      <c r="B33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="10">
+        <v>84119</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="10">
+        <v>2</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>7</v>
@@ -1428,22 +1437,24 @@
         <v>8</v>
       </c>
       <c r="E34" s="10">
-        <v>84117</v>
+        <v>84123</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="10">
-        <v>25</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>7</v>
@@ -1452,22 +1463,22 @@
         <v>8</v>
       </c>
       <c r="E35" s="10">
-        <v>84104</v>
+        <v>84115</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="10">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>7</v>
@@ -1482,30 +1493,28 @@
         <v>10</v>
       </c>
       <c r="G36" s="10">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="10">
-        <v>84106</v>
-      </c>
-      <c r="F37" s="11">
-        <v>0.4375</v>
+        <v>84121</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G37" s="10">
         <v>2</v>
@@ -1514,10 +1523,10 @@
     </row>
     <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>7</v>
@@ -1526,46 +1535,46 @@
         <v>8</v>
       </c>
       <c r="E38" s="10">
-        <v>84103</v>
-      </c>
-      <c r="F38" s="11">
-        <v>0.4375</v>
+        <v>84118</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G38" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="10">
-        <v>84119</v>
-      </c>
-      <c r="F39" s="11">
-        <v>0.4375</v>
+        <v>84107</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G39" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>7</v>
@@ -1574,24 +1583,22 @@
         <v>8</v>
       </c>
       <c r="E40" s="10">
-        <v>84119</v>
+        <v>84117</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="10">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>7</v>
@@ -1600,46 +1607,48 @@
         <v>8</v>
       </c>
       <c r="E41" s="10">
-        <v>84106</v>
+        <v>84104</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="10">
-        <v>84117</v>
-      </c>
-      <c r="F42" s="11">
-        <v>0.4375</v>
+        <v>84115</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G42" s="10">
-        <v>2</v>
-      </c>
-      <c r="H42" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>7</v>
@@ -1648,48 +1657,48 @@
         <v>8</v>
       </c>
       <c r="E43" s="10">
-        <v>84104</v>
+        <v>84119</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G43" s="10">
-        <v>88</v>
-      </c>
-      <c r="H43" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="10">
-        <v>84119</v>
+        <v>84106</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G44" s="10">
-        <v>88</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>12</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>7</v>
@@ -1698,37 +1707,37 @@
         <v>8</v>
       </c>
       <c r="E45" s="10">
-        <v>84111</v>
-      </c>
-      <c r="F45" s="11">
-        <v>0.4375</v>
+        <v>84104</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G45" s="10">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="10">
-        <v>84111</v>
+        <v>84119</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="10">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>12</v>
@@ -1736,10 +1745,10 @@
     </row>
     <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>7</v>
@@ -1748,7 +1757,7 @@
         <v>8</v>
       </c>
       <c r="E47" s="10">
-        <v>84104</v>
+        <v>84111</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>10</v>
@@ -1756,14 +1765,16 @@
       <c r="G47" s="10">
         <v>9</v>
       </c>
-      <c r="H47" s="4"/>
+      <c r="H47" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>7</v>
@@ -1772,23 +1783,24 @@
         <v>8</v>
       </c>
       <c r="E48" s="10">
-        <v>84115</v>
-      </c>
-      <c r="F48" s="11">
-        <v>0.4375</v>
+        <v>84104</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G48" s="10">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="H48" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:H48" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H48">
-      <sortCondition ref="A8:A48"/>
+      <sortCondition ref="F8:F48"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:M22">
+    <sortCondition ref="F9:F22"/>
     <sortCondition ref="A9:A22"/>
   </sortState>
   <mergeCells count="3">
@@ -1803,6 +1815,52 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2240,68 +2298,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A0206-F67A-481E-AE05-AF5EAD7E6628}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2325,9 +2325,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A0206-F67A-481E-AE05-AF5EAD7E6628}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>